<commit_message>
Finally Added Acquaintance Model
</commit_message>
<xml_diff>
--- a/SENG696 Architecture.xlsx
+++ b/SENG696 Architecture.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ispar\Desktop\SENG696_Repo\SENG696\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0F01954A-6E83-48D8-B59B-DE74395F88CB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A88C9C-6D57-4368-9A31-8E5B046BC344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{C6A042E6-D3C1-40DC-ACFB-48C7EC627BF5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{C6A042E6-D3C1-40DC-ACFB-48C7EC627BF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Role Model" sheetId="1" r:id="rId1"/>
     <sheet name="Interaction Model_x0009_" sheetId="2" r:id="rId2"/>
     <sheet name="Agent Model" sheetId="3" r:id="rId3"/>
     <sheet name="Service Model" sheetId="4" r:id="rId4"/>
+    <sheet name="Acquaintance Model" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -552,82 +553,82 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="15" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -689,6 +690,61 @@
         <a:xfrm>
           <a:off x="624840" y="373380"/>
           <a:ext cx="3634740" cy="3440971"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>7620</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>586740</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>146957</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{EDC22577-BEC5-2D41-63FC-5B49A2470ABA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="617220" y="373380"/>
+          <a:ext cx="7284720" cy="4162697"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -1014,46 +1070,46 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="23"/>
+      <c r="B1" s="37"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="12" t="s">
+      <c r="A2" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="21"/>
+      <c r="B2" s="34"/>
       <c r="C2" s="3" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="21"/>
+      <c r="B3" s="34"/>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="4" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="21"/>
+      <c r="B4" s="34"/>
       <c r="C4" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="5" spans="1:3" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="22" t="s">
+      <c r="B5" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C5" s="3" t="s">
@@ -1061,8 +1117,8 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="14"/>
-      <c r="B6" s="24" t="s">
+      <c r="A6" s="35"/>
+      <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C6" s="4" t="s">
@@ -1071,46 +1127,46 @@
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="23"/>
+      <c r="B8" s="37"/>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" s="12" t="s">
+      <c r="A9" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B9" s="21"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="3" t="s">
         <v>14</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B10" s="21"/>
+      <c r="B10" s="34"/>
       <c r="C10" s="3" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" s="12" t="s">
+      <c r="A11" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B11" s="21"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="3" t="s">
         <v>16</v>
       </c>
     </row>
     <row r="12" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B12" s="22" t="s">
+      <c r="B12" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C12" s="3" t="s">
@@ -1118,8 +1174,8 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="14"/>
-      <c r="B13" s="24" t="s">
+      <c r="A13" s="35"/>
+      <c r="B13" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C13" s="4" t="s">
@@ -1128,46 +1184,46 @@
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="23"/>
+      <c r="B15" s="37"/>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A16" s="12" t="s">
+      <c r="A16" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B16" s="21"/>
+      <c r="B16" s="34"/>
       <c r="C16" s="3" t="s">
         <v>20</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A17" s="12" t="s">
+      <c r="A17" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B17" s="21"/>
+      <c r="B17" s="34"/>
       <c r="C17" s="3" t="s">
         <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A18" s="12" t="s">
+      <c r="A18" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B18" s="21"/>
+      <c r="B18" s="34"/>
       <c r="C18" s="3" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="19" spans="1:3" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B19" s="22" t="s">
+      <c r="B19" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C19" s="3" t="s">
@@ -1175,8 +1231,8 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="14"/>
-      <c r="B20" s="24" t="s">
+      <c r="A20" s="35"/>
+      <c r="B20" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C20" s="4" t="s">
@@ -1185,46 +1241,46 @@
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="23"/>
+      <c r="B22" s="37"/>
       <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A23" s="12" t="s">
+      <c r="A23" s="33" t="s">
         <v>2</v>
       </c>
-      <c r="B23" s="21"/>
+      <c r="B23" s="34"/>
       <c r="C23" s="3" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A24" s="12" t="s">
+      <c r="A24" s="33" t="s">
         <v>4</v>
       </c>
-      <c r="B24" s="21"/>
+      <c r="B24" s="34"/>
       <c r="C24" s="3" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A25" s="12" t="s">
+      <c r="A25" s="33" t="s">
         <v>6</v>
       </c>
-      <c r="B25" s="21"/>
+      <c r="B25" s="34"/>
       <c r="C25" s="3" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A26" s="12" t="s">
+      <c r="A26" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="B26" s="22" t="s">
+      <c r="B26" s="18" t="s">
         <v>9</v>
       </c>
       <c r="C26" s="3" t="s">
@@ -1232,8 +1288,8 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="14"/>
-      <c r="B27" s="24" t="s">
+      <c r="A27" s="35"/>
+      <c r="B27" s="19" t="s">
         <v>11</v>
       </c>
       <c r="C27" s="4" t="s">
@@ -1242,14 +1298,6 @@
     </row>
   </sheetData>
   <mergeCells count="20">
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -1262,6 +1310,14 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1283,22 +1339,22 @@
     <col min="5" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="26" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="25" t="s">
+    <row r="1" spans="1:4" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="20" t="s">
         <v>31</v>
       </c>
-      <c r="B1" s="27" t="s">
+      <c r="B1" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C1" s="28" t="s">
+      <c r="C1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="29" t="s">
+      <c r="D1" s="24" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:4" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="16" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="5" t="s">
@@ -1312,7 +1368,7 @@
       </c>
     </row>
     <row r="3" spans="1:4" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="A3" s="19" t="s">
+      <c r="A3" s="16" t="s">
         <v>39</v>
       </c>
       <c r="B3" s="5" t="s">
@@ -1326,7 +1382,7 @@
       </c>
     </row>
     <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="19" t="s">
+      <c r="A4" s="16" t="s">
         <v>43</v>
       </c>
       <c r="B4" s="5" t="s">
@@ -1340,7 +1396,7 @@
       </c>
     </row>
     <row r="5" spans="1:4" s="8" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="20" t="s">
+      <c r="A5" s="17" t="s">
         <v>47</v>
       </c>
       <c r="B5" s="9" t="s">
@@ -1376,105 +1432,120 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54DEFCFB-C1DE-473B-82B7-6F7C626173F4}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="47.5546875" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.6640625" style="37" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="20.44140625" style="37" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="26.21875" style="37" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="44.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.88671875" style="37"/>
+    <col min="1" max="1" width="47.5546875" style="32" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="26.6640625" style="32" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="20.44140625" style="32" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="26.21875" style="32" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="44.33203125" style="32" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="32"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="15" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="16" t="s">
+    <row r="1" spans="1:5" s="12" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="B1" s="17" t="s">
+      <c r="B1" s="14" t="s">
         <v>52</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="14" t="s">
         <v>53</v>
       </c>
-      <c r="D1" s="17" t="s">
+      <c r="D1" s="14" t="s">
         <v>54</v>
       </c>
-      <c r="E1" s="18" t="s">
+      <c r="E1" s="15" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="2" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A2" s="30" t="s">
+    <row r="2" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A2" s="25" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="31" t="s">
+      <c r="B2" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="26" t="s">
         <v>57</v>
       </c>
-      <c r="D2" s="31" t="s">
+      <c r="D2" s="26" t="s">
         <v>58</v>
       </c>
-      <c r="E2" s="32" t="s">
+      <c r="E2" s="27" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="3" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="30" t="s">
+    <row r="3" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A3" s="25" t="s">
         <v>13</v>
       </c>
-      <c r="B3" s="31" t="s">
+      <c r="B3" s="26" t="s">
         <v>56</v>
       </c>
-      <c r="C3" s="31" t="s">
+      <c r="C3" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="31" t="s">
+      <c r="D3" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="E3" s="32" t="s">
+      <c r="E3" s="27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="4" spans="1:5" s="33" customFormat="1" x14ac:dyDescent="0.3">
-      <c r="A4" s="30" t="s">
+    <row r="4" spans="1:5" s="28" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="B4" s="31" t="s">
+      <c r="B4" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="C4" s="31" t="s">
+      <c r="C4" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="D4" s="31" t="s">
+      <c r="D4" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="27" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="5" spans="1:5" s="33" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A5" s="34" t="str">
+    <row r="5" spans="1:5" s="28" customFormat="1" ht="15" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="A5" s="29" t="str">
         <f>'Role Model'!C22</f>
         <v>Storage of Image data into a CSV data base</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="30" t="s">
         <v>68</v>
       </c>
-      <c r="C5" s="35" t="s">
+      <c r="C5" s="30" t="s">
         <v>69</v>
       </c>
-      <c r="D5" s="35" t="s">
+      <c r="D5" s="30" t="s">
         <v>70</v>
       </c>
-      <c r="E5" s="36" t="s">
+      <c r="E5" s="31" t="s">
         <v>67</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{ADE9B7B7-4E0E-4C9C-AF8E-5D95878F939C}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="O20" sqref="O20"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Basic Agent Communication added
</commit_message>
<xml_diff>
--- a/SENG696 Architecture.xlsx
+++ b/SENG696 Architecture.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ispar\Desktop\SENG696_Repo\SENG696\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70A88C9C-6D57-4368-9A31-8E5B046BC344}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{590DE04B-00D0-4AF8-A1E2-2E142F6E1561}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="4" xr2:uid="{C6A042E6-D3C1-40DC-ACFB-48C7EC627BF5}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="4" xr2:uid="{C6A042E6-D3C1-40DC-ACFB-48C7EC627BF5}"/>
   </bookViews>
   <sheets>
     <sheet name="Role Model" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="71">
   <si>
     <t>Role Schema</t>
   </si>
@@ -620,13 +620,13 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1055,8 +1055,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19741D7B-9483-43E4-B8CD-DD516D543BD5}">
   <dimension ref="A1:C27"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+    <sheetView topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="A22" sqref="A22:C27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1070,10 +1070,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37"/>
+      <c r="B1" s="36"/>
       <c r="C1" s="1" t="s">
         <v>1</v>
       </c>
@@ -1117,7 +1117,7 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A6" s="35"/>
+      <c r="A6" s="37"/>
       <c r="B6" s="19" t="s">
         <v>11</v>
       </c>
@@ -1127,10 +1127,10 @@
     </row>
     <row r="7" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" s="36" t="s">
+      <c r="A8" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B8" s="37"/>
+      <c r="B8" s="36"/>
       <c r="C8" s="1" t="s">
         <v>13</v>
       </c>
@@ -1174,7 +1174,7 @@
       </c>
     </row>
     <row r="13" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="35"/>
+      <c r="A13" s="37"/>
       <c r="B13" s="19" t="s">
         <v>11</v>
       </c>
@@ -1184,10 +1184,10 @@
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A15" s="36" t="s">
+      <c r="A15" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B15" s="37"/>
+      <c r="B15" s="36"/>
       <c r="C15" s="1" t="s">
         <v>19</v>
       </c>
@@ -1231,7 +1231,7 @@
       </c>
     </row>
     <row r="20" spans="1:3" ht="29.4" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A20" s="35"/>
+      <c r="A20" s="37"/>
       <c r="B20" s="19" t="s">
         <v>11</v>
       </c>
@@ -1241,10 +1241,10 @@
     </row>
     <row r="21" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35"/>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A22" s="36" t="s">
+      <c r="A22" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B22" s="37"/>
+      <c r="B22" s="36"/>
       <c r="C22" s="1" t="s">
         <v>25</v>
       </c>
@@ -1288,7 +1288,7 @@
       </c>
     </row>
     <row r="27" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A27" s="35"/>
+      <c r="A27" s="37"/>
       <c r="B27" s="19" t="s">
         <v>11</v>
       </c>
@@ -1298,6 +1298,14 @@
     </row>
   </sheetData>
   <mergeCells count="20">
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="A26:A27"/>
+    <mergeCell ref="A17:B17"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="A19:A20"/>
+    <mergeCell ref="A22:B22"/>
+    <mergeCell ref="A23:B23"/>
+    <mergeCell ref="A24:B24"/>
     <mergeCell ref="A16:B16"/>
     <mergeCell ref="A1:B1"/>
     <mergeCell ref="A2:B2"/>
@@ -1310,14 +1318,6 @@
     <mergeCell ref="A11:B11"/>
     <mergeCell ref="A12:A13"/>
     <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="A26:A27"/>
-    <mergeCell ref="A17:B17"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="A19:A20"/>
-    <mergeCell ref="A22:B22"/>
-    <mergeCell ref="A23:B23"/>
-    <mergeCell ref="A24:B24"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -1326,20 +1326,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{969D6C4B-3826-4FA6-8350-29BB20A05701}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" width="17.88671875" style="2" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.109375" style="2" customWidth="1"/>
     <col min="3" max="3" width="34.44140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="27.33203125" style="2" customWidth="1"/>
-    <col min="5" max="16384" width="8.88671875" style="2"/>
+    <col min="4" max="4" width="17.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.33203125" style="2" customWidth="1"/>
+    <col min="6" max="16384" width="8.88671875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="21" customFormat="1" ht="21" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="20" t="s">
         <v>31</v>
       </c>
@@ -1349,11 +1352,14 @@
       <c r="C1" s="23" t="s">
         <v>33</v>
       </c>
-      <c r="D1" s="24" t="s">
+      <c r="D1" s="20" t="s">
+        <v>31</v>
+      </c>
+      <c r="E1" s="24" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="2" spans="1:4" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:5" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="16" t="s">
         <v>35</v>
       </c>
@@ -1363,11 +1369,14 @@
       <c r="C2" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="D2" s="7" t="s">
+      <c r="D2" s="16" t="s">
+        <v>35</v>
+      </c>
+      <c r="E2" s="7" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="3" spans="1:4" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:5" s="8" customFormat="1" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="16" t="s">
         <v>39</v>
       </c>
@@ -1377,11 +1386,14 @@
       <c r="C3" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="D3" s="7" t="s">
+      <c r="D3" s="16" t="s">
+        <v>39</v>
+      </c>
+      <c r="E3" s="7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="4" spans="1:4" s="8" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:5" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A4" s="16" t="s">
         <v>43</v>
       </c>
@@ -1391,11 +1403,14 @@
       <c r="C4" s="6" t="s">
         <v>45</v>
       </c>
-      <c r="D4" s="7" t="s">
+      <c r="D4" s="16" t="s">
+        <v>43</v>
+      </c>
+      <c r="E4" s="7" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="5" spans="1:4" s="8" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" s="8" customFormat="1" ht="58.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A5" s="17" t="s">
         <v>47</v>
       </c>
@@ -1405,7 +1420,10 @@
       <c r="C5" s="10" t="s">
         <v>49</v>
       </c>
-      <c r="D5" s="11" t="s">
+      <c r="D5" s="17" t="s">
+        <v>47</v>
+      </c>
+      <c r="E5" s="11" t="s">
         <v>50</v>
       </c>
     </row>
@@ -1419,7 +1437,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7E650D45-D985-4103-B262-5FDF7DA67E9B}">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
@@ -1432,7 +1452,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{54DEFCFB-C1DE-473B-82B7-6F7C626173F4}">
   <dimension ref="A1:E5"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" activeCellId="1" sqref="A1:A5 D1:E5"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>

</xml_diff>